<commit_message>
vault backup: 2025-12-24 20:29:07
</commit_message>
<xml_diff>
--- a/10-areas/Relationships/Divorce/Respondent (Mark)/Court Documents/Final/20251224 - Form ES2.xlsx
+++ b/10-areas/Relationships/Divorce/Respondent (Mark)/Court Documents/Final/20251224 - Form ES2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A11B86F7-7AF0-A649-9716-4264F6EB3D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76464328-B206-5443-A729-36061F3F4179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32960" yWindow="2920" windowWidth="34340" windowHeight="26460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,6 +41,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8246D13E-B757-2548-88AB-327372DBDF26}</author>
+  </authors>
+  <commentList>
+    <comment ref="I139" authorId="0" shapeId="0" xr:uid="{8246D13E-B757-2548-88AB-327372DBDF26}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In my view, since you pay this off every month in full I don't think this is an enduring liability.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="96">
   <si>
@@ -348,7 +366,7 @@
     <numFmt numFmtId="169" formatCode="0.0000"/>
     <numFmt numFmtId="170" formatCode="#,##0.0000_);\(#,##0.0000\)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -447,6 +465,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1617,11 +1641,47 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="9" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="6" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="11" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="6" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -1629,21 +1689,60 @@
     <xf numFmtId="6" fontId="5" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="6" fontId="9" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="6" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="6" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="6" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1661,81 +1760,6 @@
     </xf>
     <xf numFmtId="6" fontId="11" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="9" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="11" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1796,6 +1820,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2083,16 +2111,24 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I139" dT="2025-12-24T20:26:35.21" personId="{00000000-0000-0000-0000-000000000000}" id="{8246D13E-B757-2548-88AB-327372DBDF26}">
+    <text>In my view, since you pay this off every month in full I don't think this is an enduring liability.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="55" workbookViewId="0">
-      <pane ySplit="16" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="16" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M134" sqref="M134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2113,10 +2149,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="4" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="210" t="s">
+      <c r="A1" s="238" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="210"/>
+      <c r="B1" s="238"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="139" t="s">
@@ -2124,15 +2160,15 @@
       </c>
       <c r="F1" s="140"/>
       <c r="G1" s="141"/>
-      <c r="H1" s="231" t="s">
+      <c r="H1" s="223" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="232"/>
+      <c r="I1" s="224"/>
       <c r="J1" s="141"/>
-      <c r="K1" s="231" t="s">
+      <c r="K1" s="223" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="233"/>
+      <c r="L1" s="225"/>
       <c r="M1" s="3"/>
       <c r="O1" s="5"/>
     </row>
@@ -2146,17 +2182,17 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="211">
+      <c r="H2" s="218">
         <f>SUM(E55+H55+K55)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="212"/>
+      <c r="I2" s="222"/>
       <c r="J2" s="10"/>
-      <c r="K2" s="211">
+      <c r="K2" s="218">
         <f>SUM(F55+I55+L55)</f>
         <v>0</v>
       </c>
-      <c r="L2" s="234"/>
+      <c r="L2" s="219"/>
       <c r="M2" s="3"/>
       <c r="O2" s="3"/>
     </row>
@@ -2174,17 +2210,17 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="211">
+      <c r="H3" s="218">
         <f>SUM(E73+H73+K73)</f>
         <v>64.36</v>
       </c>
-      <c r="I3" s="212"/>
+      <c r="I3" s="222"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="211">
+      <c r="K3" s="218">
         <f>SUM(F73+I73+L73)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="234"/>
+      <c r="L3" s="219"/>
       <c r="M3" s="3"/>
       <c r="O3" s="3"/>
     </row>
@@ -2192,27 +2228,27 @@
       <c r="A4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="235" t="s">
+      <c r="B4" s="216" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="235"/>
-      <c r="D4" s="236"/>
+      <c r="C4" s="216"/>
+      <c r="D4" s="217"/>
       <c r="E4" s="7" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="211">
+      <c r="H4" s="218">
         <f>SUM(E85+H85+K85)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="212"/>
+      <c r="I4" s="222"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="211">
+      <c r="K4" s="218">
         <f>SUM(F85+I85+L85)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="234"/>
+      <c r="L4" s="219"/>
       <c r="M4" s="3"/>
       <c r="O4" s="3"/>
     </row>
@@ -2220,27 +2256,27 @@
       <c r="A5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="235" t="s">
+      <c r="B5" s="216" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="235"/>
-      <c r="D5" s="236"/>
+      <c r="C5" s="216"/>
+      <c r="D5" s="217"/>
       <c r="E5" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="211">
+      <c r="H5" s="218">
         <f>SUM(E95+H95+K95)</f>
         <v>15.84</v>
       </c>
-      <c r="I5" s="212"/>
+      <c r="I5" s="222"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="211">
+      <c r="K5" s="218">
         <f>SUM(F95+I95+L95)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="234"/>
+      <c r="L5" s="219"/>
       <c r="M5" s="3"/>
       <c r="O5" s="3"/>
     </row>
@@ -2254,17 +2290,17 @@
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="211">
+      <c r="H6" s="218">
         <f>SUM(E107+H107+K107)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="212"/>
+      <c r="I6" s="222"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="211">
+      <c r="K6" s="218">
         <f>SUM(F107+I107+L107)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="234"/>
+      <c r="L6" s="219"/>
       <c r="M6" s="3"/>
       <c r="O6" s="3"/>
     </row>
@@ -2276,17 +2312,17 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="211">
+      <c r="H7" s="218">
         <f>SUM(E119+H119+K119)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="212"/>
+      <c r="I7" s="222"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="211">
+      <c r="K7" s="218">
         <f>SUM(F119+I119+L119)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="234"/>
+      <c r="L7" s="219"/>
       <c r="M7" s="3"/>
       <c r="O7" s="3"/>
     </row>
@@ -2304,17 +2340,17 @@
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="208">
+      <c r="H8" s="220">
         <f>SUM(E144+H144+K144)</f>
         <v>-69033</v>
       </c>
-      <c r="I8" s="213"/>
+      <c r="I8" s="239"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="208">
+      <c r="K8" s="220">
         <f>SUM(F144+I144+L144)</f>
         <v>-1211.95</v>
       </c>
-      <c r="L8" s="209"/>
+      <c r="L8" s="221"/>
       <c r="M8" s="3"/>
       <c r="O8" s="3"/>
     </row>
@@ -2332,17 +2368,17 @@
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="214">
+      <c r="H9" s="209">
         <f>SUM(H2:I8)</f>
         <v>-68952.800000000003</v>
       </c>
-      <c r="I9" s="215"/>
+      <c r="I9" s="240"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="214">
+      <c r="K9" s="209">
         <f>SUM(K2:L8)</f>
         <v>-1211.95</v>
       </c>
-      <c r="L9" s="237"/>
+      <c r="L9" s="210"/>
       <c r="M9" s="3"/>
       <c r="O9" s="3"/>
     </row>
@@ -2352,11 +2388,11 @@
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="216"/>
-      <c r="I10" s="217"/>
+      <c r="H10" s="241"/>
+      <c r="I10" s="242"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="238"/>
-      <c r="L10" s="239"/>
+      <c r="K10" s="211"/>
+      <c r="L10" s="212"/>
       <c r="M10" s="3"/>
       <c r="O10" s="3"/>
     </row>
@@ -2374,17 +2410,17 @@
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="208">
+      <c r="H11" s="220">
         <f>SUM(E159+H159)</f>
         <v>161237.70000000001</v>
       </c>
-      <c r="I11" s="213"/>
+      <c r="I11" s="239"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="208">
+      <c r="K11" s="220">
         <f>SUM(F159+I159)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="209"/>
+      <c r="L11" s="221"/>
       <c r="M11" s="3"/>
       <c r="O11" s="3"/>
     </row>
@@ -2398,17 +2434,17 @@
       </c>
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="218">
+      <c r="H12" s="243">
         <f>H9+H11</f>
         <v>92284.900000000009</v>
       </c>
-      <c r="I12" s="220"/>
+      <c r="I12" s="245"/>
       <c r="J12" s="21"/>
-      <c r="K12" s="218">
+      <c r="K12" s="243">
         <f>K9+K11</f>
         <v>-1211.95</v>
       </c>
-      <c r="L12" s="219"/>
+      <c r="L12" s="244"/>
       <c r="M12" s="3"/>
       <c r="O12" s="3"/>
     </row>
@@ -2435,20 +2471,20 @@
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
-      <c r="E14" s="240" t="s">
+      <c r="E14" s="213" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="241"/>
+      <c r="F14" s="214"/>
       <c r="G14" s="25"/>
-      <c r="H14" s="240" t="s">
+      <c r="H14" s="213" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="241"/>
+      <c r="I14" s="214"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="240" t="s">
+      <c r="K14" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="242"/>
+      <c r="L14" s="215"/>
       <c r="M14" s="164"/>
     </row>
     <row r="15" spans="1:15" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.15">
@@ -3356,7 +3392,7 @@
       <c r="A60" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B60" s="245">
+      <c r="B60" s="208">
         <v>73252671</v>
       </c>
       <c r="C60" s="82"/>
@@ -3376,7 +3412,7 @@
       <c r="A61" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="245">
+      <c r="B61" s="208">
         <v>93994880</v>
       </c>
       <c r="C61" s="82"/>
@@ -3397,7 +3433,7 @@
       <c r="A62" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="245" t="s">
+      <c r="B62" s="208" t="s">
         <v>86</v>
       </c>
       <c r="C62" s="82"/>
@@ -3418,7 +3454,7 @@
       <c r="A63" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="245" t="s">
+      <c r="B63" s="208" t="s">
         <v>87</v>
       </c>
       <c r="C63" s="82"/>
@@ -3439,7 +3475,7 @@
       <c r="A64" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="245" t="s">
+      <c r="B64" s="208" t="s">
         <v>91</v>
       </c>
       <c r="C64" s="82"/>
@@ -3460,7 +3496,7 @@
       <c r="A65" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="B65" s="245" t="s">
+      <c r="B65" s="208" t="s">
         <v>92</v>
       </c>
       <c r="C65" s="82"/>
@@ -3481,7 +3517,7 @@
       <c r="A66" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="B66" s="245" t="s">
+      <c r="B66" s="208" t="s">
         <v>93</v>
       </c>
       <c r="C66" s="82"/>
@@ -4729,8 +4765,8 @@
       <c r="E139" s="32"/>
       <c r="F139" s="46"/>
       <c r="G139" s="53"/>
-      <c r="H139" s="243"/>
-      <c r="I139" s="244">
+      <c r="H139" s="206"/>
+      <c r="I139" s="207">
         <v>-1211.95</v>
       </c>
       <c r="J139" s="53"/>
@@ -4847,20 +4883,20 @@
       <c r="B146" s="108"/>
       <c r="C146" s="199"/>
       <c r="D146" s="199"/>
-      <c r="E146" s="206" t="s">
+      <c r="E146" s="236" t="s">
         <v>56</v>
       </c>
-      <c r="F146" s="207"/>
+      <c r="F146" s="237"/>
       <c r="G146" s="109"/>
-      <c r="H146" s="206" t="s">
+      <c r="H146" s="236" t="s">
         <v>57</v>
       </c>
-      <c r="I146" s="207"/>
+      <c r="I146" s="237"/>
       <c r="J146" s="109"/>
-      <c r="K146" s="206" t="s">
-        <v>0</v>
-      </c>
-      <c r="L146" s="207"/>
+      <c r="K146" s="236" t="s">
+        <v>0</v>
+      </c>
+      <c r="L146" s="237"/>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A147" s="110"/>
@@ -4958,15 +4994,15 @@
       <c r="B151" s="161"/>
       <c r="C151" s="194"/>
       <c r="D151" s="189"/>
-      <c r="E151" s="224" t="s">
+      <c r="E151" s="229" t="s">
         <v>56</v>
       </c>
-      <c r="F151" s="225"/>
+      <c r="F151" s="230"/>
       <c r="G151" s="61"/>
-      <c r="H151" s="224" t="s">
+      <c r="H151" s="229" t="s">
         <v>57</v>
       </c>
-      <c r="I151" s="225"/>
+      <c r="I151" s="230"/>
       <c r="J151" s="61"/>
       <c r="K151" s="106"/>
       <c r="L151" s="106"/>
@@ -5156,20 +5192,20 @@
       <c r="B162" s="170"/>
       <c r="C162" s="203"/>
       <c r="D162" s="203"/>
-      <c r="E162" s="227" t="s">
+      <c r="E162" s="232" t="s">
         <v>56</v>
       </c>
-      <c r="F162" s="228"/>
+      <c r="F162" s="233"/>
       <c r="G162" s="171"/>
-      <c r="H162" s="227" t="s">
+      <c r="H162" s="232" t="s">
         <v>57</v>
       </c>
-      <c r="I162" s="228"/>
+      <c r="I162" s="233"/>
       <c r="J162" s="171"/>
-      <c r="K162" s="229" t="s">
-        <v>0</v>
-      </c>
-      <c r="L162" s="230"/>
+      <c r="K162" s="234" t="s">
+        <v>0</v>
+      </c>
+      <c r="L162" s="235"/>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A163" s="172"/>
@@ -5278,18 +5314,18 @@
       <c r="B168" s="163"/>
       <c r="C168" s="194"/>
       <c r="D168" s="194"/>
-      <c r="E168" s="224" t="s">
+      <c r="E168" s="229" t="s">
         <v>56</v>
       </c>
-      <c r="F168" s="225"/>
+      <c r="F168" s="230"/>
       <c r="G168" s="61"/>
-      <c r="H168" s="224" t="s">
+      <c r="H168" s="229" t="s">
         <v>57</v>
       </c>
-      <c r="I168" s="225"/>
+      <c r="I168" s="230"/>
       <c r="J168" s="61"/>
-      <c r="K168" s="226"/>
-      <c r="L168" s="226"/>
+      <c r="K168" s="231"/>
+      <c r="L168" s="231"/>
       <c r="M168" s="168"/>
     </row>
     <row r="169" spans="1:13" s="122" customFormat="1" x14ac:dyDescent="0.15">
@@ -5533,17 +5569,17 @@
       <c r="B183" s="53"/>
       <c r="C183" s="53"/>
       <c r="D183" s="53"/>
-      <c r="E183" s="221" t="s">
+      <c r="E183" s="226" t="s">
         <v>20</v>
       </c>
-      <c r="F183" s="222"/>
+      <c r="F183" s="227"/>
       <c r="G183" s="53"/>
-      <c r="H183" s="221" t="s">
+      <c r="H183" s="226" t="s">
         <v>20</v>
       </c>
-      <c r="I183" s="222"/>
-      <c r="K183" s="223"/>
-      <c r="L183" s="223"/>
+      <c r="I183" s="227"/>
+      <c r="K183" s="228"/>
+      <c r="L183" s="228"/>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A184" s="53"/>
@@ -5570,34 +5606,6 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="E183:F183"/>
-    <mergeCell ref="H183:I183"/>
-    <mergeCell ref="K183:L183"/>
-    <mergeCell ref="E151:F151"/>
-    <mergeCell ref="H151:I151"/>
-    <mergeCell ref="E168:F168"/>
-    <mergeCell ref="H168:I168"/>
-    <mergeCell ref="K168:L168"/>
-    <mergeCell ref="E162:F162"/>
-    <mergeCell ref="H162:I162"/>
-    <mergeCell ref="K162:L162"/>
     <mergeCell ref="E146:F146"/>
     <mergeCell ref="H146:I146"/>
     <mergeCell ref="K146:L146"/>
@@ -5614,6 +5622,34 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="E183:F183"/>
+    <mergeCell ref="H183:I183"/>
+    <mergeCell ref="K183:L183"/>
+    <mergeCell ref="E151:F151"/>
+    <mergeCell ref="H151:I151"/>
+    <mergeCell ref="E168:F168"/>
+    <mergeCell ref="H168:I168"/>
+    <mergeCell ref="K168:L168"/>
+    <mergeCell ref="E162:F162"/>
+    <mergeCell ref="H162:I162"/>
+    <mergeCell ref="K162:L162"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K14:L14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.86614173228346458" right="0.47244094488188981" top="0.70866141732283472" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5621,5 +5657,6 @@
   <headerFooter differentFirst="1" alignWithMargins="0">
     <firstHeader>&amp;C&amp;"Arial,Bold"TEMPLATE ES2</firstHeader>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>